<commit_message>
big ole example run done
</commit_message>
<xml_diff>
--- a/output/out_2023-10-30T15:44:08.636/params/params_2.xlsx
+++ b/output/out_2023-10-30T15:44:08.636/params/params_2.xlsx
@@ -422,22 +422,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.34288292259397146</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E2">
         <v>0.2</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>2.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>